<commit_message>
table additions to the supplementary text
</commit_message>
<xml_diff>
--- a/tables/table_03_v2.xlsx
+++ b/tables/table_03_v2.xlsx
@@ -29,15 +29,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="9">
   <si>
-    <t>MOI_50</t>
-  </si>
-  <si>
-    <t>MOI_500</t>
-  </si>
-  <si>
-    <t>MOI_5000</t>
-  </si>
-  <si>
     <t>Sample size</t>
   </si>
   <si>
@@ -54,6 +45,15 @@
   </si>
   <si>
     <t>Infection time</t>
+  </si>
+  <si>
+    <t>MOI 50</t>
+  </si>
+  <si>
+    <t>MOI 500</t>
+  </si>
+  <si>
+    <t>MOI 5000</t>
   </si>
 </sst>
 </file>
@@ -209,6 +209,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -218,7 +219,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,12 +499,12 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" style="10" bestFit="1" customWidth="1"/>
@@ -513,27 +513,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>4</v>
+      <c r="A1" s="12" t="s">
+        <v>1</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
+      <c r="A2" s="13"/>
       <c r="B2" s="4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -549,9 +549,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="4" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5">
         <v>0.66</v>
@@ -567,9 +567,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C4" s="5">
         <v>0.24</v>
@@ -585,9 +585,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5" s="8">
         <v>92</v>
@@ -601,27 +601,27 @@
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>5</v>
+      <c r="A6" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
@@ -637,9 +637,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="4" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C8" s="5">
         <v>0.09</v>
@@ -655,9 +655,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C9" s="5">
         <v>0</v>
@@ -673,9 +673,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C10" s="8">
         <v>92</v>
@@ -689,27 +689,27 @@
       <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>6</v>
+      <c r="A11" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
@@ -725,9 +725,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="4" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C13" s="5">
         <v>0</v>
@@ -743,9 +743,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C14" s="5">
         <v>0</v>
@@ -761,9 +761,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C15" s="8">
         <v>92</v>
@@ -777,27 +777,27 @@
       <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
-        <v>7</v>
+      <c r="A16" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
@@ -813,9 +813,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="4" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C18" s="5">
         <v>0.02</v>
@@ -831,9 +831,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C19" s="5">
         <v>0</v>
@@ -849,9 +849,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C20" s="8">
         <v>92</v>
@@ -865,27 +865,27 @@
       <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
-        <v>8</v>
+      <c r="A21" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="12"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C22" s="5">
         <v>1</v>
@@ -901,9 +901,9 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="4" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C23" s="5">
         <v>0</v>
@@ -919,9 +919,9 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C24" s="5">
         <v>0</v>
@@ -937,9 +937,9 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C25" s="8">
         <v>92</v>

</xml_diff>